<commit_message>
Updated the POVBase to use a PSoC, it is about the same price as a 555 and more flexible.
</commit_message>
<xml_diff>
--- a/POVDisplayRotate/MPQ4420 calculator.xlsx
+++ b/POVDisplayRotate/MPQ4420 calculator.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
   <si>
     <t>Vout</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>Ceramic Delta Vout</t>
+  </si>
+  <si>
+    <t>L ripple current</t>
   </si>
 </sst>
 </file>
@@ -145,10 +148,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,7 +460,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -479,7 +483,7 @@
       </c>
       <c r="B4">
         <f>B3/B2</f>
-        <v>0.14285714285714285</v>
+        <v>0.15625</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -529,10 +533,11 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9">
-        <v>0.4</v>
+        <v>26</v>
+      </c>
+      <c r="B9" s="3">
+        <f>B3*(B2-B3)/(B2*B8*B11)</f>
+        <v>1.0289634146341462</v>
       </c>
       <c r="C9" t="s">
         <v>12</v>
@@ -540,82 +545,93 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B10">
-        <v>410000</v>
+        <v>0.4</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B11">
-        <f>B9*SQRT(B4*(1-B4))</f>
-        <v>0.13997084244475305</v>
+        <v>410000</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="2">
-        <v>1E-4</v>
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <f>B10*SQRT(B4*(1-B4))</f>
+        <v>0.14523687548277814</v>
       </c>
       <c r="C12" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B13" s="2">
-        <v>0.01</v>
+        <v>1E-4</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14">
-        <f>(B9/(B10*0.000022))*B4*(1-B4)</f>
-        <v>5.4301099597266851E-3</v>
+        <v>23</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0.01</v>
       </c>
       <c r="C14" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="2">
-        <f>B3/(B10*B8)*(1-B4)*(B13+(1/(8*B10*B12)))</f>
-        <v>1.3639840231154924E-2</v>
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <f>(B10/(B11*0.000022))*B4*(1-B4)</f>
+        <v>5.8463830376940138E-3</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="2">
+        <f>B3/(B11*B8)*(1-B4)*(B14+(1/(8*B11*B13)))</f>
+        <v>1.3426717727543128E-2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>25</v>
       </c>
-      <c r="B17">
-        <f>B3/(8*POWER(B10,2)*B8*B12)*(1-B4)</f>
-        <v>3.1868785586810573E-3</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="B18">
+        <f>B3/(8*POWER(B11,2)*B8*B13)*(1-B4)</f>
+        <v>3.1370835812016655E-3</v>
+      </c>
+      <c r="C18" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>